<commit_message>
#update water spider detail
</commit_message>
<xml_diff>
--- a/ME-API/Resources/Template/SME_Score_Record_Detail_Template.xlsx
+++ b/ME-API/Resources/Template/SME_Score_Record_Detail_Template.xlsx
@@ -189,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -218,6 +218,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -503,7 +506,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:F1"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,13 +586,13 @@
     </row>
     <row r="4" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="D4" s="13"/>
       <c r="E4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="13"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>

</xml_diff>